<commit_message>
US Consumer Discretionary naming change.
</commit_message>
<xml_diff>
--- a/Transactions_sample.xlsx
+++ b/Transactions_sample.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zahitevrenkaya/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zahitevrenkaya/Workspace/portfolio_viewer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{670505D2-2E9A-2D4E-A3BC-85EA08D0FD57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5B36E41-214A-374F-B246-AE5555D2C78F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3080" yWindow="2100" windowWidth="27840" windowHeight="16740" xr2:uid="{9087DB79-7593-FD45-AC56-002D37809B2C}"/>
   </bookViews>
@@ -152,10 +152,10 @@
     <t>Nike</t>
   </si>
   <si>
-    <t>Stock - Consumer Discretionary</t>
-  </si>
-  <si>
     <t>US Stock Consumer Discretionary</t>
+  </si>
+  <si>
+    <t>Stock - US Consumer Discretionary</t>
   </si>
 </sst>
 </file>
@@ -569,7 +569,7 @@
   <dimension ref="A1:Z12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -844,10 +844,10 @@
         <v>37</v>
       </c>
       <c r="C12" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>38</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>39</v>
       </c>
       <c r="E12" s="4">
         <v>45546</v>

</xml_diff>